<commit_message>
bugfix num_impressions and policy report outputs
</commit_message>
<xml_diff>
--- a/auction_ini_01.xlsx
+++ b/auction_ini_01.xlsx
@@ -195,14 +195,14 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -210,7 +210,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="n">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>1</v>
@@ -221,7 +221,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>12345</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>